<commit_message>
#42 LAB-5 fix report - add grid and fix figure
</commit_message>
<xml_diff>
--- a/documents/Lab4/report15th.xlsx
+++ b/documents/Lab4/report15th.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Gdansk University of Technology\sixth_semester\LargeScaleEnterpriseApplication\Lab\Repository\single_sign_on\documents\Lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E220BC-2194-49B6-83AC-7A7FF369F983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402CA54E-AF11-4520-AF20-2EE93813461D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis - Longest Logs" sheetId="1" r:id="rId1"/>
@@ -269,6 +269,13 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -306,6 +313,13 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -334,10 +348,6 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="tr"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
@@ -527,6 +537,13 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -564,6 +581,13 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -592,10 +616,6 @@
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="tr"/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
     <c:showDLblsOverMax val="1"/>
@@ -990,7 +1010,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1134,7 +1154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>